<commit_message>
refactor. maxHP -> stamina.
</commit_message>
<xml_diff>
--- a/Documents/ExcelData/EnemyData.xlsx
+++ b/Documents/ExcelData/EnemyData.xlsx
@@ -27,9 +27,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>maxHP</t>
-  </si>
-  <si>
     <t>power</t>
   </si>
   <si>
@@ -90,6 +87,10 @@
   </si>
   <si>
     <t>isBoss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stamina</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -419,7 +420,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -438,49 +439,49 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
       <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
@@ -488,13 +489,13 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -541,13 +542,13 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>2500</v>
+        <v>99</v>
       </c>
       <c r="E3">
         <v>25</v>
@@ -594,13 +595,13 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>9999</v>
+        <v>255</v>
       </c>
       <c r="E4">
         <v>99</v>

</xml_diff>

<commit_message>
add specialized weapon, magic and skill to enemy.
</commit_message>
<xml_diff>
--- a/Documents/ExcelData/EnemyData.xlsx
+++ b/Documents/ExcelData/EnemyData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>name</t>
   </si>
@@ -67,22 +67,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ring1ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ring2ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>黑·咩咩</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>真·爱新觉萝莉</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>isBoss</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -163,10 +147,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>戒指ID1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>是否BOSS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -175,7 +155,99 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>戒指ID2</t>
+    <t>暴走澪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>山神咩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>法术ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>道具ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>magicIDs</t>
+  </si>
+  <si>
+    <t>itemKeys</t>
+  </si>
+  <si>
+    <t>itemValues</t>
+  </si>
+  <si>
+    <t>道具数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>4002,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>400</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>400</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>002</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -183,7 +255,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -197,6 +269,12 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="宋体"/>
       <family val="3"/>
@@ -231,14 +309,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -521,233 +605,247 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="8.625" customWidth="1"/>
-    <col min="11" max="11" width="10.5" customWidth="1"/>
-    <col min="14" max="14" width="11.625" customWidth="1"/>
+    <col min="3" max="4" width="8.625" customWidth="1"/>
+    <col min="12" max="12" width="10.5" customWidth="1"/>
+    <col min="16" max="16" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.75" customWidth="1"/>
+    <col min="18" max="18" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>40</v>
+      <c r="Q3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>14</v>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A4" s="3">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0</v>
+      </c>
+      <c r="R4" s="3">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A4" s="1">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1">
-        <v>0</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>10</v>
       </c>
@@ -758,7 +856,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E5" s="2">
         <v>10</v>
@@ -782,92 +880,90 @@
         <v>10</v>
       </c>
       <c r="L5" s="2">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <v>2</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
       <c r="O5" s="2">
-        <v>0</v>
+        <v>3001</v>
       </c>
       <c r="P5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0</v>
-      </c>
+        <v>4001</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
         <v>99</v>
       </c>
-      <c r="E6" s="2">
-        <v>25</v>
-      </c>
       <c r="F6" s="2">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G6" s="2">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H6" s="2">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="I6" s="2">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="J6" s="2">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="K6" s="2">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="L6" s="2">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2">
-        <v>0</v>
-      </c>
-      <c r="P6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>0</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
         <v>255</v>
-      </c>
-      <c r="E7" s="2">
-        <v>99</v>
       </c>
       <c r="F7" s="2">
         <v>99</v>
@@ -888,23 +984,17 @@
         <v>99</v>
       </c>
       <c r="L7" s="2">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0</v>
-      </c>
-      <c r="N7" s="2">
-        <v>1</v>
-      </c>
-      <c r="O7" s="2">
-        <v>0</v>
-      </c>
-      <c r="P7" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>0</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Bugfix and balance tweak. Also save game after battle.
</commit_message>
<xml_diff>
--- a/Documents/ExcelData/EnemyData.xlsx
+++ b/Documents/ExcelData/EnemyData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="127">
   <si>
     <t>name</t>
   </si>
@@ -669,6 +669,18 @@
   </si>
   <si>
     <t>Both</t>
+  </si>
+  <si>
+    <t>99</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>255</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1087,7 +1099,7 @@
   <dimension ref="A1:R59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -1487,8 +1499,8 @@
       <c r="E8" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F8" s="2">
-        <v>99</v>
+      <c r="F8" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="G8" s="2">
         <v>50</v>
@@ -1515,8 +1527,12 @@
         <v>3002</v>
       </c>
       <c r="O8" s="2"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
+      <c r="P8" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>1</v>
+      </c>
       <c r="R8" s="4" t="s">
         <v>119</v>
       </c>
@@ -1534,11 +1550,11 @@
       <c r="D9" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F9" s="2">
-        <v>255</v>
+      <c r="E9" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="G9" s="2">
         <v>99</v>
@@ -1565,8 +1581,12 @@
       <c r="O9" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
+      <c r="P9" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="R9" s="4" t="s">
         <v>119</v>
       </c>

</xml_diff>